<commit_message>
Sync SharePoint -> GitHub (Liste Agents.xlsx)
</commit_message>
<xml_diff>
--- a/Liste Agents.xlsx
+++ b/Liste Agents.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29721"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sncf-my.sharepoint.com/personal/0500182b_commun_ad_sncf_fr/Documents/Bureau/Logiciel/Formation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{D060550D-EC24-4B93-998A-76DB785E2407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{94039DB2-997E-4D4F-93D7-CECE235F1FEE}"/>
+  <xr:revisionPtr revIDLastSave="72" documentId="8_{D060550D-EC24-4B93-998A-76DB785E2407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8290D6FD-948B-4392-B06B-EF1D441A2653}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="10520" windowWidth="19180" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="20">
   <si>
     <t>Nom agent</t>
   </si>
@@ -66,28 +66,31 @@
     <t>PRM4</t>
   </si>
   <si>
+    <t>12h - 20h</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>OUI</t>
+  </si>
+  <si>
+    <t>NON</t>
+  </si>
+  <si>
+    <t>Léa</t>
+  </si>
+  <si>
+    <t>PRM11</t>
+  </si>
+  <si>
+    <t>Brann</t>
+  </si>
+  <si>
     <t xml:space="preserve">04h - 12h </t>
   </si>
   <si>
     <t>A</t>
-  </si>
-  <si>
-    <t>OUI</t>
-  </si>
-  <si>
-    <t>NON</t>
-  </si>
-  <si>
-    <t>Léa</t>
-  </si>
-  <si>
-    <t>MR2</t>
-  </si>
-  <si>
-    <t>12h - 20h</t>
-  </si>
-  <si>
-    <t>B</t>
   </si>
   <si>
     <t>Vacation</t>
@@ -100,8 +103,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -129,8 +140,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -149,8 +161,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{086EF4FB-C52F-4436-BE29-1FB47AED532C}" name="Tableau1" displayName="Tableau1" ref="A1:G3" totalsRowShown="0">
-  <autoFilter ref="A1:G3" xr:uid="{086EF4FB-C52F-4436-BE29-1FB47AED532C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{086EF4FB-C52F-4436-BE29-1FB47AED532C}" name="Tableau1" displayName="Tableau1" ref="A1:G5" totalsRowShown="0">
+  <autoFilter ref="A1:G5" xr:uid="{086EF4FB-C52F-4436-BE29-1FB47AED532C}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{482C4117-9B84-4166-ABBA-78057EA6DE48}" name="Nom agent"/>
     <tableColumn id="7" xr3:uid="{D67EA537-E6E8-426E-A4AD-7C4FB539B6C3}" name="Zone"/>
@@ -165,9 +177,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -205,7 +217,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -311,7 +323,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -453,7 +465,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -461,13 +473,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.28515625" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" customWidth="1"/>
@@ -475,7 +487,7 @@
     <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -498,7 +510,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -521,7 +533,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -529,19 +541,42 @@
         <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s">
         <v>11</v>
       </c>
       <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
         <v>11</v>
       </c>
-      <c r="G3" t="s">
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
         <v>12</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -559,19 +594,19 @@
           <x14:formula1>
             <xm:f>data!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C3</xm:sqref>
+          <xm:sqref>C2:C5</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7650F547-F190-4B3E-BAF3-AE887D4DC04D}">
           <x14:formula1>
             <xm:f>data!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D3</xm:sqref>
+          <xm:sqref>D2:D5</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{98964C5C-C68E-4CD2-820D-7616F37176D5}">
           <x14:formula1>
             <xm:f>data!$C$1:$C$2</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:G3</xm:sqref>
+          <xm:sqref>E2:G5</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -587,47 +622,299 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010074E679F04C92FB4FBFCFE144A70329CD" ma:contentTypeVersion="15" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="4f54f62f668ae452afbf95b08919f63a">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="812cf66e-8db3-4c80-a76c-da518b79a7be" xmlns:ns3="636cb9cc-9200-44e7-b82d-7956be2d2b7a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="61e6388f1c5eb5c7c75ddc111675a703" ns2:_="" ns3:_="">
+    <xsd:import namespace="812cf66e-8db3-4c80-a76c-da518b79a7be"/>
+    <xsd:import namespace="636cb9cc-9200-44e7-b82d-7956be2d2b7a"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns2:_Flow_SignoffStatus" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="812cf66e-8db3-4c80-a76c-da518b79a7be" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="10" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="11" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="12" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="13" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="14" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="16" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Balises d’images" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="5096f5d6-3256-4090-9362-038d665d1958" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="18" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="19" nillable="true" ma:displayName="Location" ma:indexed="true" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="20" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="21" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="_Flow_SignoffStatus" ma:index="22" nillable="true" ma:displayName="État de validation" ma:internalName="_x0024_Resources_x003a_core_x002c_Signoff_Status">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="636cb9cc-9200-44e7-b82d-7956be2d2b7a" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="TaxCatchAll" ma:index="17" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{92193ee3-1a87-4a7c-902a-77b8e348e808}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="636cb9cc-9200-44e7-b82d-7956be2d2b7a">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Type de contenu"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Titre"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="812cf66e-8db3-4c80-a76c-da518b79a7be">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="636cb9cc-9200-44e7-b82d-7956be2d2b7a" xsi:nil="true"/>
+    <_Flow_SignoffStatus xmlns="812cf66e-8db3-4c80-a76c-da518b79a7be" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6B9030D-C2DA-4563-B33A-03E57CA2F85A}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77570D1F-F189-415B-A6E7-2AB0AB0E6B1A}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{295E16E5-F136-485F-A80A-C48D5A0E37BB}"/>
 </file>
</xml_diff>